<commit_message>
Updates to Fig 3
</commit_message>
<xml_diff>
--- a/Phase_Field_Fracture/Figures/LengthTest.xlsx
+++ b/Phase_Field_Fracture/Figures/LengthTest.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idaang/Documents/GitHub/FEniCS/Phase_Field_Fracture/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idaang/Documents/GitHub/FEniCS/Phase_Field_Fracture/Figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDF8E90-E174-4342-8492-FECC61B0D9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E39DA63-0AB7-BF47-BC01-DA7F7C2CC6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="500" windowWidth="20480" windowHeight="15140" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4220" yWindow="600" windowWidth="18760" windowHeight="15140" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExpLoad" sheetId="1" r:id="rId1"/>
     <sheet name="Task2_Prelim" sheetId="2" r:id="rId2"/>
     <sheet name="Task2" sheetId="3" r:id="rId3"/>
-    <sheet name="Task3" sheetId="4" r:id="rId4"/>
-    <sheet name="Task4-3D" sheetId="5" r:id="rId5"/>
+    <sheet name="Summary" sheetId="6" r:id="rId4"/>
+    <sheet name="Task3" sheetId="4" r:id="rId5"/>
+    <sheet name="Task4-3D" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="135">
   <si>
     <t>Delta</t>
   </si>
@@ -431,6 +432,18 @@
   </si>
   <si>
     <t>Using same setup as below, just extended the number of steps</t>
+  </si>
+  <si>
+    <t>Delta_p (Gc_e)</t>
+  </si>
+  <si>
+    <t>Delta_p (Gc)</t>
+  </si>
+  <si>
+    <t>Delta %E (Gc)</t>
+  </si>
+  <si>
+    <t>Delta %E (Gc_e)</t>
   </si>
 </sst>
 </file>
@@ -450,7 +463,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -517,6 +530,30 @@
         <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFCD3C1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED7D31"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C6E7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C6E7"/>
+        <bgColor rgb="FFFCD3C1"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -530,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -552,6 +589,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -561,10 +602,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1046,7 +1092,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="A6" sqref="A6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2389,22 +2435,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AJ31"/>
+  <dimension ref="A1:AJ35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection sqref="A1:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="4.1640625" customWidth="1"/>
-    <col min="3" max="3" width="5.5" customWidth="1"/>
+    <col min="2" max="2" width="5.5" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="5" width="5" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="8.5" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.1640625" customWidth="1"/>
     <col min="10" max="11" width="11.5"/>
     <col min="12" max="12" width="13.6640625" customWidth="1"/>
@@ -2444,10 +2490,10 @@
         <v>7</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>14</v>
+        <v>132</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>131</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>0</v>
@@ -2456,10 +2502,10 @@
         <v>24</v>
       </c>
       <c r="K1" t="s">
-        <v>25</v>
+        <v>133</v>
       </c>
       <c r="L1" t="s">
-        <v>26</v>
+        <v>134</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>8</v>
@@ -2553,18 +2599,18 @@
         <v>9.4106153860191171</v>
       </c>
       <c r="L2">
-        <f t="shared" ref="L2:L10" si="1">ABS(H2-J2)/H2*100</f>
+        <f t="shared" ref="L2:L11" si="1">ABS(H2-J2)/H2*100</f>
         <v>6.5375766256943439</v>
       </c>
       <c r="M2">
         <v>0.02</v>
       </c>
       <c r="N2">
-        <f t="shared" ref="N2:N10" si="2">5*M2</f>
+        <f t="shared" ref="N2:N11" si="2">5*M2</f>
         <v>0.1</v>
       </c>
       <c r="O2">
-        <f t="shared" ref="O2:O10" si="3">20*M2</f>
+        <f t="shared" ref="O2:O11" si="3">20*M2</f>
         <v>0.4</v>
       </c>
       <c r="P2" t="s">
@@ -2577,15 +2623,15 @@
         <v>41</v>
       </c>
       <c r="T2">
-        <f t="shared" ref="T2:T10" si="4">M2</f>
+        <f t="shared" ref="T2:T11" si="4">M2</f>
         <v>0.02</v>
       </c>
       <c r="W2">
-        <f t="shared" ref="W2:W10" si="5">6/T2</f>
+        <f t="shared" ref="W2:W11" si="5">6/T2</f>
         <v>300</v>
       </c>
       <c r="X2">
-        <f t="shared" ref="X2:X10" si="6">1/T2</f>
+        <f t="shared" ref="X2:X11" si="6">1/T2</f>
         <v>50</v>
       </c>
       <c r="Y2" t="s">
@@ -2613,7 +2659,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C10" si="7">B3*(1+(3/2)*M3/N3)</f>
+        <f t="shared" ref="C3:C11" si="7">B3*(1+(3/2)*M3/N3)</f>
         <v>1.3</v>
       </c>
       <c r="D3" s="5">
@@ -3350,74 +3396,117 @@
       <c r="AI10" s="2"/>
       <c r="AJ10" s="2"/>
     </row>
-    <row r="11" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2"/>
-      <c r="Y11" s="2"/>
-      <c r="Z11" s="2"/>
-      <c r="AA11" s="2"/>
-      <c r="AB11" s="2"/>
-      <c r="AC11" s="2"/>
-      <c r="AD11" s="2"/>
-      <c r="AE11" s="2"/>
-      <c r="AF11" s="2"/>
-      <c r="AG11" s="2"/>
-      <c r="AH11" s="2"/>
-      <c r="AI11" s="2"/>
-      <c r="AJ11" s="2"/>
+    <row r="11" spans="1:36" s="27" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="20">
+        <v>1</v>
+      </c>
+      <c r="B11" s="20">
+        <v>1</v>
+      </c>
+      <c r="C11" s="20">
+        <f t="shared" si="7"/>
+        <v>1.3</v>
+      </c>
+      <c r="D11" s="26">
+        <f>100000</f>
+        <v>100000</v>
+      </c>
+      <c r="E11" s="20">
+        <v>6</v>
+      </c>
+      <c r="F11" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="27">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="H11" s="20">
+        <v>0.5454</v>
+      </c>
+      <c r="I11" s="20">
+        <v>0.53</v>
+      </c>
+      <c r="J11" s="26"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="28">
+        <f>ABS(H11-J11)/H11*100</f>
+        <v>100</v>
+      </c>
+      <c r="M11" s="20">
+        <v>2E-3</v>
+      </c>
+      <c r="N11" s="20">
+        <f t="shared" si="2"/>
+        <v>0.01</v>
+      </c>
+      <c r="O11" s="20">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="P11" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q11" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="R11" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="S11" s="20">
+        <v>300</v>
+      </c>
+      <c r="T11" s="20">
+        <f t="shared" si="4"/>
+        <v>2E-3</v>
+      </c>
+      <c r="U11" s="20"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="20">
+        <f t="shared" si="5"/>
+        <v>3000</v>
+      </c>
+      <c r="X11" s="20">
+        <f t="shared" si="6"/>
+        <v>500</v>
+      </c>
+      <c r="Y11" s="20"/>
+      <c r="Z11" s="20"/>
+      <c r="AA11" s="20"/>
+      <c r="AB11" s="20"/>
+      <c r="AC11" s="20"/>
+      <c r="AD11" s="20"/>
+      <c r="AE11" s="20"/>
+      <c r="AF11" s="20"/>
+      <c r="AG11" s="20"/>
+      <c r="AH11" s="20"/>
+      <c r="AI11" s="20"/>
+      <c r="AJ11" s="20"/>
     </row>
     <row r="12" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19">
-        <f>20*M12</f>
-        <v>0</v>
-      </c>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="19"/>
-      <c r="U12" s="19"/>
-      <c r="V12" s="19"/>
-      <c r="W12" s="19"/>
-      <c r="X12" s="11"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
@@ -3431,534 +3520,507 @@
       <c r="AI12" s="2"/>
       <c r="AJ12" s="2"/>
     </row>
-    <row r="13" spans="1:36" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2">
-        <f t="shared" ref="C13:C14" si="8">B13*(1+(3/2)*M13/N13)</f>
+    <row r="13" spans="1:36" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23">
+        <f>20*M13</f>
+        <v>0</v>
+      </c>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="23"/>
+      <c r="W13" s="23"/>
+      <c r="X13" s="11"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2"/>
+      <c r="AH13" s="2"/>
+      <c r="AI13" s="2"/>
+      <c r="AJ13" s="2"/>
+    </row>
+    <row r="14" spans="1:36" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" ref="C14:C15" si="8">B14*(1+(3/2)*M14/N14)</f>
         <v>1.3</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D14" s="5">
         <v>100001</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>6</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <v>0.5</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>0.46589999999999998</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H14" s="2">
         <v>0.5454</v>
       </c>
-      <c r="I13">
+      <c r="I14">
         <v>0.53</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J14" s="5">
         <v>0.52197689202699504</v>
       </c>
-      <c r="K13">
-        <f>ABS(G13-J13)/G13*100</f>
+      <c r="K14">
+        <f>ABS(G14-J14)/G14*100</f>
         <v>12.036250703368763</v>
       </c>
-      <c r="L13">
-        <f>ABS(H13-J13)/H13*100</f>
+      <c r="L14">
+        <f>ABS(H14-J14)/H14*100</f>
         <v>4.2946659283104056</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M14" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="N13" s="2">
-        <f>5*M13</f>
+      <c r="N14" s="2">
+        <f>5*M14</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="O13">
-        <f>20*M13</f>
+      <c r="O14">
+        <f>20*M14</f>
         <v>0.1</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="P14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="Q14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="R13" s="8" t="s">
+      <c r="R14" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="S13" s="12">
+      <c r="S14" s="12">
         <v>250</v>
       </c>
-      <c r="T13">
-        <f>M13</f>
+      <c r="T14">
+        <f>M14</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="U13">
+      <c r="U14">
         <v>0.15</v>
       </c>
-      <c r="V13">
+      <c r="V14">
         <v>0.15</v>
       </c>
-      <c r="W13">
-        <f>6/T13</f>
+      <c r="W14">
+        <f>6/T14</f>
         <v>1200</v>
       </c>
-      <c r="X13">
-        <f>1/T13</f>
+      <c r="X14">
+        <f>1/T14</f>
         <v>200</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="Y14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:36" s="15" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="15">
-        <v>1</v>
-      </c>
-      <c r="B14" s="15">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2">
+    <row r="15" spans="1:36" s="15" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="15">
+        <v>1</v>
+      </c>
+      <c r="B15" s="15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
         <f t="shared" si="8"/>
         <v>1.3</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D15" s="17">
         <v>100001</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E15" s="15">
         <v>6</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F15" s="15">
         <v>0.5</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G15" s="15">
         <v>0.46589999999999998</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H15" s="2">
         <v>0.5454</v>
       </c>
-      <c r="I14" s="15">
+      <c r="I15" s="15">
         <v>0.53</v>
       </c>
-      <c r="J14" s="17">
+      <c r="J15" s="17">
         <v>0.52395329616751496</v>
       </c>
-      <c r="K14" s="15">
-        <f>ABS(G14-J14)/G14*100</f>
+      <c r="K15" s="15">
+        <f>ABS(G15-J15)/G15*100</f>
         <v>12.460462796204116</v>
       </c>
-      <c r="L14" s="15">
-        <f>ABS(H14-J14)/H14*100</f>
+      <c r="L15" s="15">
+        <f>ABS(H15-J15)/H15*100</f>
         <v>3.9322889315154081</v>
       </c>
-      <c r="M14" s="15">
+      <c r="M15" s="15">
         <v>2E-3</v>
       </c>
-      <c r="N14" s="15">
-        <f>5*M14</f>
+      <c r="N15" s="15">
+        <f>5*M15</f>
         <v>0.01</v>
       </c>
-      <c r="O14" s="15">
-        <f>20*M14</f>
+      <c r="O15" s="15">
+        <f>20*M15</f>
         <v>0.04</v>
       </c>
-      <c r="P14" s="15" t="s">
+      <c r="P15" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="Q14" s="15" t="s">
+      <c r="Q15" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="R14" s="15" t="s">
+      <c r="R15" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="S14" s="15">
+      <c r="S15" s="15">
         <v>300</v>
       </c>
-      <c r="T14" s="15">
-        <f>M14</f>
+      <c r="T15" s="15">
+        <f>M15</f>
         <v>2E-3</v>
       </c>
-      <c r="U14" s="15">
+      <c r="U15" s="15">
         <v>0.16</v>
       </c>
-      <c r="V14" s="15">
+      <c r="V15" s="15">
         <v>0.06</v>
       </c>
-      <c r="W14" s="15">
-        <f>6/T14</f>
+      <c r="W15" s="15">
+        <f>6/T15</f>
         <v>3000</v>
       </c>
-      <c r="X14" s="15">
-        <f>1/T14</f>
+      <c r="X15" s="15">
+        <f>1/T15</f>
         <v>500</v>
       </c>
-      <c r="Y14" s="15" t="s">
+      <c r="Y15" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.15">
-      <c r="A15" s="19" t="s">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.15">
+      <c r="A16" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="19"/>
-      <c r="S15" s="19"/>
-      <c r="T15" s="19"/>
-      <c r="U15" s="19"/>
-      <c r="V15" s="19"/>
-      <c r="W15" s="19"/>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.15">
-      <c r="A16" s="2">
-        <v>1</v>
-      </c>
-      <c r="B16" s="2">
-        <v>1</v>
-      </c>
-      <c r="C16" s="2">
-        <f t="shared" ref="C16:C17" si="9">B16*(1+(3/2)*M16/N16)</f>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="23"/>
+      <c r="W16" s="23"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A17" s="2">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" ref="C17:C18" si="9">B17*(1+(3/2)*M17/N17)</f>
         <v>1.3</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D17" s="7">
         <v>100001</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E17" s="2">
         <v>6</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F17" s="2">
         <v>0.5</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G17" s="10">
         <v>0.46589999999999998</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H17" s="2">
         <v>0.5454</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I17" s="10">
         <v>0.53</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J17" s="7">
         <v>0.519920705566292</v>
       </c>
-      <c r="K16" s="9">
-        <f>ABS(G16-J16)/G16*100</f>
+      <c r="K17" s="9">
+        <f>ABS(G17-J17)/G17*100</f>
         <v>11.594914266214213</v>
       </c>
-      <c r="L16" s="18">
-        <f t="shared" ref="L16" si="10">ABS(H16-J16)/H16*100</f>
+      <c r="L17" s="18">
+        <f t="shared" ref="L17" si="10">ABS(H17-J17)/H17*100</f>
         <v>4.671671146627796</v>
       </c>
-      <c r="M16">
+      <c r="M17">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="N16" s="10">
-        <f>5*M16</f>
+      <c r="N17" s="10">
+        <f>5*M17</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="O16" s="15">
-        <f>20*M16</f>
+      <c r="O17" s="15">
+        <f>20*M17</f>
         <v>0.1</v>
       </c>
-      <c r="S16">
+      <c r="S17">
         <v>325</v>
       </c>
-      <c r="T16" s="10">
-        <f>M16</f>
+      <c r="T17" s="10">
+        <f>M17</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="U16">
+      <c r="U17">
         <v>0.1</v>
       </c>
-      <c r="V16" t="s">
+      <c r="V17" t="s">
         <v>71</v>
       </c>
-      <c r="Z16" t="s">
+      <c r="Z17" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A17" s="10">
-        <v>1</v>
-      </c>
-      <c r="B17" s="10">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A18" s="10">
+        <v>1</v>
+      </c>
+      <c r="B18" s="10">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2">
         <f t="shared" si="9"/>
         <v>1.3</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D18" s="9">
         <v>100001</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E18" s="10">
         <v>6</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F18" s="10">
         <v>0.5</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G18" s="10">
         <v>0.46589999999999998</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H18" s="2">
         <v>0.5454</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I18" s="10">
         <v>0.53</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J18" s="9">
         <v>0.52395329616749997</v>
       </c>
-      <c r="K17" s="10">
-        <f>ABS(G17-J17)/G17*100</f>
+      <c r="K18" s="10">
+        <f>ABS(G18-J18)/G18*100</f>
         <v>12.4604627962009</v>
       </c>
-      <c r="L17" s="10">
-        <f>ABS(H17-J17)/H17*100</f>
+      <c r="L18" s="10">
+        <f>ABS(H18-J18)/H18*100</f>
         <v>3.9322889315181562</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M18" s="10">
         <v>2E-3</v>
       </c>
-      <c r="N17" s="10">
-        <f>5*M17</f>
+      <c r="N18" s="10">
+        <f>5*M18</f>
         <v>0.01</v>
       </c>
-      <c r="O17" s="10">
-        <f>20*M17</f>
+      <c r="O18" s="10">
+        <f>20*M18</f>
         <v>0.04</v>
       </c>
-      <c r="P17" s="10" t="s">
+      <c r="P18" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="Q17" s="10" t="s">
+      <c r="Q18" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="R17" s="10" t="s">
+      <c r="R18" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="S17" s="10">
+      <c r="S18" s="10">
         <v>300</v>
       </c>
-      <c r="T17" s="10">
-        <f>M17</f>
+      <c r="T18" s="10">
+        <f>M18</f>
         <v>2E-3</v>
       </c>
-      <c r="U17" s="10">
+      <c r="U18" s="10">
         <v>0.16</v>
       </c>
-      <c r="V17" s="10" t="s">
+      <c r="V18" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="W17" s="10">
-        <f>6/T17</f>
+      <c r="W18" s="10">
+        <f>6/T18</f>
         <v>3000</v>
       </c>
-      <c r="X17" s="10">
-        <f>1/T17</f>
+      <c r="X18" s="10">
+        <f>1/T18</f>
         <v>500</v>
       </c>
-      <c r="Y17" s="10" t="s">
+      <c r="Y18" s="10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A19" s="19" t="s">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A20" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="19"/>
-      <c r="S19" s="19"/>
-      <c r="T19" s="19"/>
-      <c r="U19" s="19"/>
-      <c r="V19" s="19"/>
-      <c r="W19" s="19"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="23"/>
+      <c r="U20" s="23"/>
+      <c r="V20" s="23"/>
+      <c r="W20" s="23"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
         <v>10</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>11</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>23</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="4" t="s">
+      <c r="G21" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I21" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J21" t="s">
         <v>24</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K21" t="s">
         <v>25</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L21" t="s">
         <v>26</v>
       </c>
-      <c r="M20" s="4" t="s">
+      <c r="M21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N21" t="s">
         <v>9</v>
       </c>
-      <c r="O20" t="s">
+      <c r="O21" t="s">
         <v>52</v>
       </c>
-      <c r="P20" t="s">
+      <c r="P21" t="s">
         <v>28</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="Q21" t="s">
         <v>29</v>
       </c>
-      <c r="R20" t="s">
+      <c r="R21" t="s">
         <v>30</v>
       </c>
-      <c r="S20" t="s">
-        <v>1</v>
-      </c>
-      <c r="T20" t="s">
+      <c r="S21" t="s">
+        <v>1</v>
+      </c>
+      <c r="T21" t="s">
         <v>31</v>
       </c>
-      <c r="U20" t="s">
+      <c r="U21" t="s">
         <v>32</v>
       </c>
-      <c r="V20" t="s">
+      <c r="V21" t="s">
         <v>33</v>
       </c>
-      <c r="W20" t="s">
+      <c r="W21" t="s">
         <v>34</v>
       </c>
-      <c r="X20" t="s">
+      <c r="X21" t="s">
         <v>35</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="Y21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2">
-        <f t="shared" ref="C21:C22" si="11">B21*(1+(3/2)*M21/N21)</f>
-        <v>1.3</v>
-      </c>
-      <c r="D21" s="5">
-        <v>100000</v>
-      </c>
-      <c r="E21">
-        <v>6</v>
-      </c>
-      <c r="F21">
-        <v>0.5</v>
-      </c>
-      <c r="G21">
-        <v>0.46589999999999998</v>
-      </c>
-      <c r="H21">
-        <v>0.48659999999999998</v>
-      </c>
-      <c r="I21">
-        <v>0.53</v>
-      </c>
-      <c r="J21" s="5"/>
-      <c r="K21">
-        <f>ABS(G21-J21)/G21*100</f>
-        <v>100</v>
-      </c>
-      <c r="L21">
-        <f>ABS(H21-J21)/H21*100</f>
-        <v>100</v>
-      </c>
-      <c r="M21">
-        <v>0.02</v>
-      </c>
-      <c r="N21">
-        <f>5*M21</f>
-        <v>0.1</v>
-      </c>
-      <c r="O21">
-        <f>M21*20</f>
-        <v>0.4</v>
-      </c>
-      <c r="P21" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="R21" t="s">
-        <v>41</v>
-      </c>
-      <c r="S21">
-        <v>53</v>
-      </c>
-      <c r="W21">
-        <f>E21/M21</f>
-        <v>300</v>
-      </c>
-      <c r="X21">
-        <f>F21*2/M21</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>1</v>
       </c>
@@ -3966,7 +4028,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="C22:C23" si="11">B22*(1+(3/2)*M22/N22)</f>
         <v>1.3</v>
       </c>
       <c r="D22" s="5">
@@ -3997,15 +4059,15 @@
         <v>100</v>
       </c>
       <c r="M22">
-        <v>5.0000000000000001E-3</v>
+        <v>0.02</v>
       </c>
       <c r="N22">
         <f>5*M22</f>
-        <v>2.5000000000000001E-2</v>
+        <v>0.1</v>
       </c>
       <c r="O22">
         <f>M22*20</f>
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="P22" t="s">
         <v>44</v>
@@ -4017,110 +4079,195 @@
         <v>41</v>
       </c>
       <c r="S22">
+        <v>53</v>
+      </c>
+      <c r="W22">
+        <f>E22/M22</f>
+        <v>300</v>
+      </c>
+      <c r="X22">
+        <f>F22*2/M22</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="11"/>
+        <v>1.3</v>
+      </c>
+      <c r="D23" s="5">
+        <v>100000</v>
+      </c>
+      <c r="E23">
+        <v>6</v>
+      </c>
+      <c r="F23">
+        <v>0.5</v>
+      </c>
+      <c r="G23">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="H23">
+        <v>0.48659999999999998</v>
+      </c>
+      <c r="I23">
+        <v>0.53</v>
+      </c>
+      <c r="J23" s="5"/>
+      <c r="K23">
+        <f>ABS(G23-J23)/G23*100</f>
+        <v>100</v>
+      </c>
+      <c r="L23">
+        <f>ABS(H23-J23)/H23*100</f>
+        <v>100</v>
+      </c>
+      <c r="M23">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N23">
+        <f>5*M23</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="O23">
+        <f>M23*20</f>
+        <v>0.1</v>
+      </c>
+      <c r="P23" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R23" t="s">
+        <v>41</v>
+      </c>
+      <c r="S23">
         <v>200</v>
       </c>
-      <c r="T22" s="2">
+      <c r="T23" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="U22" s="2">
+      <c r="U23" s="2">
         <v>0.2</v>
       </c>
-      <c r="V22" s="2">
+      <c r="V23" s="2">
         <v>0.1</v>
       </c>
-      <c r="W22" s="2">
-        <f>6/T22</f>
+      <c r="W23" s="2">
+        <f>6/T23</f>
         <v>1200</v>
       </c>
-      <c r="X22" s="2">
-        <f>V22*2/T22</f>
+      <c r="X23" s="2">
+        <f>V23*2/T23</f>
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="22"/>
-      <c r="S24" s="15"/>
-      <c r="T24" s="15"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
-      <c r="X24" s="2"/>
-      <c r="Y24" s="2"/>
-    </row>
-    <row r="25" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
       <c r="D25" s="7"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
       <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
       <c r="M25" s="15"/>
       <c r="N25" s="15"/>
       <c r="O25" s="15"/>
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
+      <c r="R25" s="19"/>
       <c r="S25" s="15"/>
       <c r="T25" s="15"/>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="F29" t="s">
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+    </row>
+    <row r="26" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="D26" s="7"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
+      <c r="T26" s="15"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="F30" t="s">
         <v>128</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G30" t="s">
         <v>127</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H30" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="F30" s="2">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="F31" s="2">
         <v>0.5454</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G31" s="7">
         <v>0.52098733289366195</v>
       </c>
-      <c r="H30" s="7">
+      <c r="H31" s="7">
         <v>0.519920705566292</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="E31" t="s">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="E32" t="s">
         <v>129</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G32" s="7">
         <f>L9</f>
         <v>4.4761032464866242</v>
       </c>
-      <c r="H31" s="7">
-        <f>L16</f>
+      <c r="H32" s="7">
+        <f>L17</f>
         <v>4.671671146627796</v>
       </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="E35" s="10"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A12:W12"/>
-    <mergeCell ref="A15:W15"/>
-    <mergeCell ref="A19:W19"/>
+    <mergeCell ref="A13:W13"/>
+    <mergeCell ref="A16:W16"/>
+    <mergeCell ref="A20:W20"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4132,6 +4279,378 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB0843D5-12C4-0D42-AE16-5A90BC5D5773}">
+  <dimension ref="A1:S11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.3</v>
+      </c>
+      <c r="D2">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="E2">
+        <v>0.5454</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0.51</v>
+      </c>
+      <c r="G2">
+        <v>9.4106153900000002</v>
+      </c>
+      <c r="H2">
+        <v>6.5375766259999999</v>
+      </c>
+      <c r="I2">
+        <v>0.02</v>
+      </c>
+      <c r="J2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.3</v>
+      </c>
+      <c r="D3">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="E3">
+        <v>0.5454</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.51</v>
+      </c>
+      <c r="G3">
+        <v>9.5283552900000004</v>
+      </c>
+      <c r="H3">
+        <v>6.4369990259999996</v>
+      </c>
+      <c r="I3">
+        <v>1.2E-2</v>
+      </c>
+      <c r="J3">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1.3</v>
+      </c>
+      <c r="D4">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="E4">
+        <v>0.5454</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0.52</v>
+      </c>
+      <c r="G4">
+        <v>11.6211804</v>
+      </c>
+      <c r="H4">
+        <v>4.6492336849999996</v>
+      </c>
+      <c r="I4">
+        <v>1.2E-2</v>
+      </c>
+      <c r="J4">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1.3</v>
+      </c>
+      <c r="D5">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="E5">
+        <v>0.5454</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.52</v>
+      </c>
+      <c r="G5">
+        <v>11.6627145</v>
+      </c>
+      <c r="H5">
+        <v>4.6137537789999996</v>
+      </c>
+      <c r="I5">
+        <v>0.01</v>
+      </c>
+      <c r="J5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1.3</v>
+      </c>
+      <c r="D6">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="E6">
+        <v>0.5454</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="G6">
+        <v>10.3392041</v>
+      </c>
+      <c r="H6">
+        <v>5.7443432789999997</v>
+      </c>
+      <c r="I6">
+        <v>0.01</v>
+      </c>
+      <c r="J6">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1.3</v>
+      </c>
+      <c r="D7">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="E7">
+        <v>0.5454</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.52</v>
+      </c>
+      <c r="G7">
+        <v>11.6627145</v>
+      </c>
+      <c r="H7">
+        <v>4.6137537789999996</v>
+      </c>
+      <c r="I7">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="J7">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1.3</v>
+      </c>
+      <c r="D8">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="E8">
+        <v>0.5454</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.52</v>
+      </c>
+      <c r="G8">
+        <v>11.6627145</v>
+      </c>
+      <c r="H8">
+        <v>4.6137537789999996</v>
+      </c>
+      <c r="I8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J8">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.3</v>
+      </c>
+      <c r="D9">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="E9">
+        <v>0.5454</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="G9">
+        <v>11.823853400000001</v>
+      </c>
+      <c r="H9" s="30">
+        <v>4.4761032460000001</v>
+      </c>
+      <c r="I9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A10" s="10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1.3</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="E10">
+        <v>0.5454</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="G10" s="9">
+        <v>13.1</v>
+      </c>
+      <c r="H10" s="9">
+        <v>3.38</v>
+      </c>
+      <c r="I10" s="10">
+        <v>2E-3</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A11" s="31">
+        <v>1</v>
+      </c>
+      <c r="B11" s="31">
+        <v>1</v>
+      </c>
+      <c r="C11" s="31">
+        <v>1.3</v>
+      </c>
+      <c r="D11" s="33">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="E11" s="31">
+        <v>0.5454</v>
+      </c>
+      <c r="F11" s="32"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="34">
+        <v>100</v>
+      </c>
+      <c r="I11" s="31">
+        <v>2E-3</v>
+      </c>
+      <c r="J11" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AC26"/>
   <sheetViews>
@@ -4233,14 +4752,14 @@
       <c r="W1" t="s">
         <v>68</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="X1" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="23"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.15">
       <c r="D2">
@@ -4405,75 +4924,75 @@
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.15">
-      <c r="A6" s="23">
-        <v>1</v>
-      </c>
-      <c r="B6" s="23">
+      <c r="A6" s="20">
+        <v>1</v>
+      </c>
+      <c r="B6" s="20">
         <v>1000</v>
       </c>
-      <c r="C6" s="23">
-        <v>1</v>
-      </c>
-      <c r="D6" s="23">
+      <c r="C6" s="20">
+        <v>1</v>
+      </c>
+      <c r="D6" s="20">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="20">
         <v>0.4</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="21">
         <v>8</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="20">
         <v>2</v>
       </c>
-      <c r="I6" s="24">
+      <c r="I6" s="21">
         <v>9.5</v>
       </c>
-      <c r="J6" s="23">
+      <c r="J6" s="20">
         <v>0.8</v>
       </c>
-      <c r="K6" s="24">
+      <c r="K6" s="21">
         <v>5</v>
       </c>
-      <c r="L6" s="23">
+      <c r="L6" s="20">
         <f>SQRT(K6^2-(F6/2)^2)</f>
         <v>3</v>
       </c>
-      <c r="M6" s="23">
+      <c r="M6" s="20">
         <f>I6/2+L6</f>
         <v>7.75</v>
       </c>
-      <c r="N6" s="23">
+      <c r="N6" s="20">
         <f>L6+I6/2</f>
         <v>7.75</v>
       </c>
-      <c r="O6" s="23">
+      <c r="O6" s="20">
         <f>F6/D6</f>
         <v>1000</v>
       </c>
-      <c r="P6" s="23">
+      <c r="P6" s="20">
         <f>J6/D6</f>
         <v>100</v>
       </c>
-      <c r="Q6" s="23">
+      <c r="Q6" s="20">
         <v>2.75</v>
       </c>
-      <c r="R6" s="23" t="s">
+      <c r="R6" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="S6" s="23">
+      <c r="S6" s="20">
         <v>2.5273500000000002</v>
       </c>
-      <c r="T6" s="23" t="s">
+      <c r="T6" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="U6" s="23">
+      <c r="U6" s="20">
         <v>275</v>
       </c>
-      <c r="V6" s="23" t="s">
+      <c r="V6" s="20" t="s">
         <v>70</v>
       </c>
       <c r="W6" t="s">
@@ -4757,14 +5276,14 @@
       <c r="W14" t="s">
         <v>42</v>
       </c>
-      <c r="X14" s="20" t="s">
+      <c r="X14" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="Y14" s="20"/>
-      <c r="Z14" s="20"/>
-      <c r="AA14" s="20"/>
-      <c r="AB14" s="20"/>
-      <c r="AC14" s="20"/>
+      <c r="Y14" s="24"/>
+      <c r="Z14" s="24"/>
+      <c r="AA14" s="24"/>
+      <c r="AB14" s="24"/>
+      <c r="AC14" s="24"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.15">
       <c r="Q15">
@@ -4870,14 +5389,14 @@
       <c r="W17" t="s">
         <v>42</v>
       </c>
-      <c r="X17" s="20" t="s">
+      <c r="X17" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="Y17" s="20"/>
-      <c r="Z17" s="20"/>
-      <c r="AA17" s="20"/>
-      <c r="AB17" s="20"/>
-      <c r="AC17" s="20"/>
+      <c r="Y17" s="24"/>
+      <c r="Z17" s="24"/>
+      <c r="AA17" s="24"/>
+      <c r="AB17" s="24"/>
+      <c r="AC17" s="24"/>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
@@ -5029,11 +5548,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
@@ -5274,14 +5793,14 @@
       <c r="U5" t="s">
         <v>96</v>
       </c>
-      <c r="W5" s="20" t="s">
+      <c r="W5" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="X5" s="20"/>
-      <c r="Y5" s="20"/>
-      <c r="Z5" s="20"/>
-      <c r="AA5" s="20"/>
-      <c r="AB5" s="20"/>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="24"/>
+      <c r="Z5" s="24"/>
+      <c r="AA5" s="24"/>
+      <c r="AB5" s="24"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.15">
       <c r="Q6">
@@ -5316,14 +5835,14 @@
       <c r="T7" t="s">
         <v>41</v>
       </c>
-      <c r="W7" s="20" t="s">
+      <c r="W7" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="X7" s="20"/>
-      <c r="Y7" s="20"/>
-      <c r="Z7" s="20"/>
-      <c r="AA7" s="20"/>
-      <c r="AB7" s="20"/>
+      <c r="X7" s="24"/>
+      <c r="Y7" s="24"/>
+      <c r="Z7" s="24"/>
+      <c r="AA7" s="24"/>
+      <c r="AB7" s="24"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A9">
@@ -5542,27 +6061,27 @@
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.15">
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="21"/>
-      <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="21"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="25"/>
+      <c r="V15" s="25"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.15">
       <c r="B16">
@@ -6536,79 +7055,79 @@
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A43" s="23">
-        <v>1</v>
-      </c>
-      <c r="B43" s="23">
+      <c r="A43" s="20">
+        <v>1</v>
+      </c>
+      <c r="B43" s="20">
         <v>0.2</v>
       </c>
-      <c r="C43" s="23">
+      <c r="C43" s="20">
         <v>200</v>
       </c>
-      <c r="D43" s="23">
+      <c r="D43" s="20">
         <f>(3*C43-2*B43)/(2*(B43+3*C43))</f>
         <v>0.49950016661112961</v>
       </c>
-      <c r="E43" s="23">
+      <c r="E43" s="20">
         <f>2*B43*(1+D43)</f>
         <v>0.59980006664445185</v>
       </c>
-      <c r="F43" s="23">
+      <c r="F43" s="20">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="G43" s="23">
+      <c r="G43" s="20">
         <v>0.04</v>
       </c>
-      <c r="H43" s="23">
+      <c r="H43" s="20">
         <v>0.5</v>
       </c>
-      <c r="I43" s="23">
+      <c r="I43" s="20">
         <v>0.75</v>
       </c>
-      <c r="J43" s="23">
+      <c r="J43" s="20">
         <f>-2*F43</f>
         <v>-1.6E-2</v>
       </c>
-      <c r="K43" s="23">
+      <c r="K43" s="20">
         <f>-J43*2</f>
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="L43" s="23">
+      <c r="L43" s="20">
         <f>4*F43</f>
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="M43" s="23">
+      <c r="M43" s="20">
         <f>2*F43</f>
         <v>1.6E-2</v>
       </c>
-      <c r="N43" s="23">
+      <c r="N43" s="20">
         <f>M43</f>
         <v>1.6E-2</v>
       </c>
-      <c r="O43" s="23">
+      <c r="O43" s="20">
         <f>I43/F43</f>
         <v>93.75</v>
       </c>
-      <c r="P43" s="23">
+      <c r="P43" s="20">
         <f>L43/F43</f>
         <v>4</v>
       </c>
-      <c r="Q43" s="25">
+      <c r="Q43" s="22">
         <v>3</v>
       </c>
-      <c r="R43" s="25">
+      <c r="R43" s="22">
         <v>2.7591999999999999</v>
       </c>
-      <c r="S43" s="25">
+      <c r="S43" s="22">
         <v>300</v>
       </c>
-      <c r="T43" s="25" t="s">
+      <c r="T43" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="U43" s="25" t="s">
+      <c r="U43" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="V43" s="25" t="s">
+      <c r="V43" s="22" t="s">
         <v>47</v>
       </c>
       <c r="W43" t="s">

</xml_diff>